<commit_message>
events module endup last touches
</commit_message>
<xml_diff>
--- a/tmp/report.xlsx
+++ b/tmp/report.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Lista de asistencia Ola amigos este es un evento" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Lista de asistencia Evento 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,36 +453,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>DIEGO BELTRAN LOPEZ</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>C20211959</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>ING.SIST.COMP.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>26/05/2024 18:11:28</t>
-        </is>
-      </c>
-      <c r="E2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Administrador d d</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
cambio de metodo get events
</commit_message>
<xml_diff>
--- a/tmp/report.xlsx
+++ b/tmp/report.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Lista de asistencia Evento 3" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Lista de asistencia hola" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -456,30 +456,30 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DIEGO BELTRAN LOPEZ</t>
+          <t>Samuel Hiram Castro Martinez</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C20211959</t>
+          <t>20212390</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>ING.SIST.COMP.</t>
+          <t>ING SISTEMAS</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>28/05/2024 21:19:02</t>
+          <t>04/07/2024 14:42:46</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Diego Beltran Lopez</t>
+          <t>Samuel Castro Martinez</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
endpoints for default data creation
</commit_message>
<xml_diff>
--- a/tmp/report.xlsx
+++ b/tmp/report.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Lista de asistencia Evento 3" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Lista de asistencia Staff Innovatec 2025" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -456,12 +456,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DIEGO BELTRAN LOPEZ</t>
+          <t>ANTHONY ALAN MATA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>C20211959</t>
+          <t>20211810</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -471,15 +471,15 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>28/05/2024 21:19:02</t>
+          <t>29/05/2024 18:11:29</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Diego Beltran Lopez</t>
+          <t>Laura Angelica Cegobiano Garcia</t>
         </is>
       </c>
     </row>

</xml_diff>